<commit_message>
Add Numerical Method New Assignment
</commit_message>
<xml_diff>
--- a/Analisis Peubah Ganda/Tugas 10-221911069-3SI1-Bill Van Ricardo Zalukhu/National Track Records for Women.xlsx
+++ b/Analisis Peubah Ganda/Tugas 10-221911069-3SI1-Bill Van Ricardo Zalukhu/National Track Records for Women.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c12dd32435a2c59/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7c12dd32435a2c59/Documents/3SI1/Semester 6/Tugas Matkul/tugas_matkul/Analisis Peubah Ganda/Tugas 10-221911069-3SI1-Bill Van Ricardo Zalukhu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ADEAA28C-5D3B-45AF-A470-F84E4E8E994C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{ADEAA28C-5D3B-45AF-A470-F84E4E8E994C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DC3C15D-643D-42F3-B654-9E0B3B19DB98}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{A3CDCF4E-E872-46D5-9C06-79AB9541269A}"/>
   </bookViews>
@@ -1553,7 +1553,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="9.109375" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">

</xml_diff>